<commit_message>
Task Completion font Standardized for CurrentWork input
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Repair San Antonio Road Bridge</t>
+    <t>Probation Camp Scudder Admin Building</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>04/29/2021</t>
+    <t>04/30/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>FA461020F0129</t>
+    <t>P-12810-90125B1</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -1341,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="13">
-        <v>6165</v>
+        <v>6208</v>
       </c>
       <c r="G3" s="14"/>
     </row>

</xml_diff>

<commit_message>
time inputmask export inprogress
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>MacArthur Park New Restroom</t>
+    <t>Test Name</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>05/05/2021</t>
+    <t>05/04/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>30J0049.00</t>
+    <t>9999999999</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,10 +52,13 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
+    <t xml:space="preserve">08 : </t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>WEATHER</t>
   </si>
   <si>
     <t xml:space="preserve">END TIME </t>
@@ -138,18 +141,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -672,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -726,13 +723,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,9 +762,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,7 +825,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1341,7 +1332,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="13">
-        <v>6249</v>
+        <v>999999</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -1354,311 +1345,311 @@
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="25" t="s">
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28" t="s">
+      <c r="C6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="D6" s="26"/>
+      <c r="E6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="33" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36"/>
+      <c r="D7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
-      <c r="M9" s="51"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="50"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-    </row>
-    <row r="16" ht="24.75" customHeight="1" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54">
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
+      <c r="A17" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
+      <c r="A18" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="63"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="68"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
       <c r="N19" s="1"/>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="68"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="66"/>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="71"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="69"/>
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="62"/>
+      <c r="A22" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
       <c r="N22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="65"/>
+      <c r="A23" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="63"/>
       <c r="N23" s="1"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="68"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="66"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="68"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="66"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69"/>
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
+      <c r="A27" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
       <c r="N27" s="1"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
+      <c r="A28" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
       <c r="N28" s="1"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="68"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="66"/>
       <c r="N29" s="1"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="66"/>
       <c r="N30" s="1"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="74"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="72"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1668,7 +1659,7 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1678,7 +1669,7 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="75"/>
+      <c r="A34" s="73"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1688,7 +1679,7 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1698,7 +1689,7 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1708,7 +1699,7 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="75"/>
+      <c r="A37" s="73"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
in case of 00 for hh unit
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t>20:00</t>
+    <t>06:00</t>
   </si>
   <si>
     <t>WEATHER</t>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>19:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -1366,26 +1369,26 @@
         <v>14</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="20"/>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="29"/>
     </row>
@@ -1393,10 +1396,10 @@
       <c r="A7" s="15"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
@@ -1477,7 +1480,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="52">
@@ -1494,7 +1497,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -1546,7 +1549,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -1597,7 +1600,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>

</xml_diff>

<commit_message>
12 hh exception complete
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t>06:00</t>
+    <t>00:10</t>
   </si>
   <si>
     <t>WEATHER</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">END TIME </t>
   </si>
   <si>
-    <t>19:00</t>
+    <t>12:30</t>
   </si>
   <si>
     <t>CONTRACTOR</t>

</xml_diff>

<commit_message>
input and font size standardized
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Test Name</t>
+    <t>DBH Landscape (East)</t>
   </si>
   <si>
     <t>DATE</t>
@@ -37,7 +37,7 @@
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>9999999999</t>
+    <t>J500010.00</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,19 +52,13 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t xml:space="preserve">7:00 </t>
+    <t/>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t xml:space="preserve">END TIME </t>
-  </si>
-  <si>
-    <t>17:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -1335,7 +1329,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="13">
-        <v>999999</v>
+        <v>6220</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -1361,34 +1355,34 @@
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G5" s="20"/>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="29"/>
     </row>
@@ -1396,10 +1390,10 @@
       <c r="A7" s="15"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
@@ -1480,7 +1474,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="52">
@@ -1497,7 +1491,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -1509,7 +1503,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" s="62"/>
       <c r="C18" s="62"/>
@@ -1549,7 +1543,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -1561,7 +1555,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="62"/>
       <c r="C23" s="62"/>
@@ -1600,7 +1594,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
@@ -1612,7 +1606,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="62"/>
       <c r="C28" s="62"/>

</xml_diff>

<commit_message>
input For Time revert
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>MacArthur Park New Restroom</t>
+    <t>Test Name</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>05/05/2021</t>
+    <t>05/04/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>30J0049.00</t>
+    <t>9999999999</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,13 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
+    <t>07:30</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>WEATHER</t>
-  </si>
-  <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>12:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -138,18 +144,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -672,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -726,13 +726,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,9 +765,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,7 +828,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1341,7 +1335,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="13">
-        <v>6249</v>
+        <v>999999</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -1354,311 +1348,311 @@
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="E5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="F5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28" t="s">
+      <c r="B6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="C6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="26"/>
+      <c r="E6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
-      <c r="M9" s="51"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="50"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-    </row>
-    <row r="16" ht="24.75" customHeight="1" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54">
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
+      <c r="A17" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
+      <c r="A18" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="63"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="68"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
       <c r="N19" s="1"/>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="68"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="66"/>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="71"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="69"/>
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="62"/>
+      <c r="A22" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
       <c r="N22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="65"/>
+      <c r="A23" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="63"/>
       <c r="N23" s="1"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="68"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="66"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="68"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="66"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69"/>
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
+      <c r="A27" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
       <c r="N27" s="1"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
+      <c r="A28" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
       <c r="N28" s="1"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="68"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="66"/>
       <c r="N29" s="1"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="66"/>
       <c r="N30" s="1"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="74"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="72"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1668,7 +1662,7 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1678,7 +1672,7 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="75"/>
+      <c r="A34" s="73"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1688,7 +1682,7 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1698,7 +1692,7 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1708,7 +1702,7 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="75"/>
+      <c r="A37" s="73"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
pdf file create complete
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>CFS Willowbrook Comp Child Ctr Fire Sprinkler System</t>
+    <t>KHS Westside Tree Shrubs</t>
   </si>
   <si>
     <t>DATE</t>
@@ -37,7 +37,7 @@
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>P-12810-90081B1</t>
+    <t>J500015.00</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -83,10 +83,13 @@
 /Day</t>
   </si>
   <si>
-    <t>Exbon Development Inc</t>
-  </si>
-  <si>
-    <t>XL Fire Protection</t>
+    <t>BrightView Landscape Services</t>
+  </si>
+  <si>
+    <t>rteertwt wrt fg afsg dfg ert eart awrt wrt wtar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> taw rtawrt awrt awrt awrt awrt awrt awrt wrt wrt wrt</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -1086,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>6146</v>
+        <v>6254</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1159,37 +1162,25 @@
         <v>11</v>
       </c>
       <c r="C8" s="30">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D8" s="31">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="35">
-        <v>3</v>
-      </c>
-      <c r="D9" s="36">
-        <v>0</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="34"/>
       <c r="L9" s="38"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,7 +1233,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="41">
@@ -1258,7 +1249,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -1305,7 +1296,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -1351,7 +1342,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>

</xml_diff>

<commit_message>
failed to export pdf on Linux
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>KHS Westside Tree Shrubs</t>
+    <t>Desert HS Modernization</t>
   </si>
   <si>
     <t>DATE</t>
@@ -37,7 +37,7 @@
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>J500015.00</t>
+    <t>17502.40</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -81,15 +81,6 @@
   <si>
     <t xml:space="preserve">HOURS
 /Day</t>
-  </si>
-  <si>
-    <t>BrightView Landscape Services</t>
-  </si>
-  <si>
-    <t>rteertwt wrt fg afsg dfg ert eart awrt wrt wtar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> taw rtawrt awrt awrt awrt awrt awrt awrt wrt wrt wrt</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -1089,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>6254</v>
+        <v>5976</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1155,24 +1146,12 @@
       <c r="F7" s="25"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="30">
-        <v>0</v>
-      </c>
-      <c r="D8" s="31">
-        <v>0</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>23</v>
-      </c>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
@@ -1233,7 +1212,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="41">
@@ -1249,7 +1228,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -1296,7 +1275,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -1342,7 +1321,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>

</xml_diff>

<commit_message>
export a tag location changed
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -31,7 +31,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>05/10/2021</t>
+    <t>05/03/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
@@ -52,13 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t/>
+    <t>07:00</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
+    <t>Sunny</t>
+  </si>
+  <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>16:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -83,16 +89,46 @@
 /Day</t>
   </si>
   <si>
+    <t>Exbon Development Inc.</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t>JPUS</t>
+  </si>
+  <si>
+    <t>Laborer</t>
+  </si>
+  <si>
+    <t>Dump Truck</t>
+  </si>
+  <si>
+    <t>Existing Partition Removal</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>TESTS &amp; INSPECTIONS</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspection is scheduled on May 4, 2021 at 3PM. </t>
+  </si>
+  <si>
     <t>CORRECTIONAL ITEMS</t>
   </si>
   <si>
+    <t>New frosted panel has a crack. Needs to be replaced.</t>
+  </si>
+  <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>All punchwork need to be performed during off-hours.</t>
   </si>
 </sst>
 </file>
@@ -1104,62 +1140,86 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="25"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="29"/>
+      <c r="A8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="30">
+        <v>2</v>
+      </c>
+      <c r="D8" s="31">
+        <v>4</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="34"/>
+      <c r="A9" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="35">
+        <v>2</v>
+      </c>
+      <c r="D9" s="36">
+        <v>4</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="L9" s="38"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1272,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="41">
@@ -1228,7 +1288,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -1239,7 +1299,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
@@ -1275,7 +1335,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -1286,7 +1346,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
@@ -1321,7 +1381,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>
@@ -1332,7 +1392,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>

</xml_diff>

<commit_message>
complete on May 11
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet sheetId="135" name="Daily Report" state="visible" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Sneeze Partition Installation</t>
+    <t>Test Name</t>
   </si>
   <si>
     <t>DATE</t>
@@ -37,7 +37,7 @@
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>9055-017.00.01</t>
+    <t>9999999999</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,13 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
+    <t>08:15</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>WEATHER</t>
-  </si>
-  <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>19:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -84,9 +90,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>TESTS &amp; INSPECTIONS</t>
@@ -105,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm AM/PM;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -122,19 +125,16 @@
     <font>
       <b/>
       <family val="2"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <family val="2"/>
-      <sz val="8"/>
-      <name val="Arial"/>
+      <scheme val="minor"/>
+      <sz val="20"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <family val="2"/>
+      <scheme val="minor"/>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -471,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -486,157 +486,166 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -660,12 +669,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1213908" cy="352425"/>
+    <xdr:ext cx="1476375" cy="428625"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1">
@@ -1027,12 +1036,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
@@ -1077,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>6261</v>
+        <v>999999</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1101,270 +1110,271 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" ht="36.75" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="F6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" ht="21" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="33"/>
-      <c r="L9" s="37"/>
-    </row>
-    <row r="10" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="33"/>
-    </row>
-    <row r="11" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="33"/>
-    </row>
-    <row r="12" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="33"/>
-    </row>
-    <row r="14" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="33"/>
-    </row>
-    <row r="15" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="33"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="34"/>
+      <c r="L9" s="38"/>
+    </row>
+    <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="34"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="34"/>
+    </row>
+    <row r="12" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="34"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="34"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="M16" s="42"/>
+      <c r="A16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41">
+        <f>SUM(C8:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="M16" s="45"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45"/>
+      <c r="A17" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="48"/>
+      <c r="A18" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="51"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="54"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="54"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="45"/>
+      <c r="A22" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="48"/>
+      <c r="A23" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="54"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="54"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="45"/>
+      <c r="A27" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="48"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
+      <c r="A28" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="54"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="54"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1373,7 +1383,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1382,7 +1392,7 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1391,7 +1401,7 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1400,7 +1410,7 @@
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1409,7 +1419,7 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Self Timesheet in progress
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet sheetId="135" name="Daily Report" state="visible" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Test Name</t>
+    <t>Sneeze Partition Installation</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>05/11/2021</t>
+    <t>05/03/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>9999999999</t>
+    <t>9055-017.00.01</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,19 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t>08:15</t>
+    <t>07:00</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
-    <t/>
+    <t>Sunny</t>
   </si>
   <si>
     <t xml:space="preserve">END TIME </t>
   </si>
   <si>
-    <t>19:00</t>
+    <t>16:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -89,16 +89,49 @@
 /Day</t>
   </si>
   <si>
+    <t>Exbon Development Inc.</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t>JPUS</t>
+  </si>
+  <si>
+    <t>Laborer</t>
+  </si>
+  <si>
+    <t>Dump Truck</t>
+  </si>
+  <si>
+    <t>Existing Partition Removal</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>TESTS &amp; INSPECTIONS</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspection is scheduled on May 4, 2021 at 3PM. </t>
+  </si>
+  <si>
     <t>CORRECTIONAL ITEMS</t>
   </si>
   <si>
+    <t>New frosted panel has a crack. Needs to be replaced.</t>
+  </si>
+  <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>All punchwork need to be performed during off-hours.</t>
   </si>
 </sst>
 </file>
@@ -108,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm AM/PM;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -125,16 +158,19 @@
     <font>
       <b/>
       <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="20"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <family val="2"/>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
       <family val="2"/>
-      <scheme val="minor"/>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -471,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -486,166 +522,157 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -669,12 +696,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1476375" cy="428625"/>
+    <xdr:ext cx="1213908" cy="352425"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1">
@@ -1036,12 +1063,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
@@ -1086,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>999999</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1125,256 +1152,279 @@
       <c r="A6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26" t="s">
+    <row r="7" ht="36.75" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="34"/>
-      <c r="L9" s="38"/>
-    </row>
-    <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="34"/>
-    </row>
-    <row r="13" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="34"/>
-    </row>
-    <row r="14" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="34"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="34"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30">
+        <v>4</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" ht="21" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="34">
+        <v>2</v>
+      </c>
+      <c r="D9" s="35">
+        <v>4</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="37"/>
+    </row>
+    <row r="10" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="33"/>
+    </row>
+    <row r="11" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="33"/>
+    </row>
+    <row r="12" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="33"/>
+    </row>
+    <row r="13" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41">
-        <f>SUM(C8:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="M16" s="45"/>
+      <c r="A16" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="M16" s="42"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
+      <c r="A17" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="45"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
+      <c r="A18" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="54"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="57"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="54"/>
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
+      <c r="A22" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="51"/>
+      <c r="A23" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="48"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="54"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="51"/>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48"/>
+      <c r="A27" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
+      <c r="A28" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="48"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="54"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="51"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="58"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1383,7 +1433,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1392,7 +1442,7 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="58"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1401,7 +1451,7 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1410,7 +1460,7 @@
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1419,7 +1469,7 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
+      <c r="A37" s="55"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Work Activities Portrait view
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Test Name</t>
+    <t>Sneeze Partition Installation</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>05/25/2021</t>
+    <t>05/03/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>9999999999</t>
+    <t>9055-017.00.01</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,13 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t/>
+    <t>05:00</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
+    <t>Sunny</t>
+  </si>
+  <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>16:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -83,16 +89,46 @@
 /Day</t>
   </si>
   <si>
+    <t>Exbon Development Inc.</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t>JPUS</t>
+  </si>
+  <si>
+    <t>Laborer</t>
+  </si>
+  <si>
+    <t>Dump Truck</t>
+  </si>
+  <si>
+    <t>Existing Partition Removal</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>TESTS &amp; INSPECTIONS</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspection is scheduled on May 4, 2021 at 3PM. </t>
+  </si>
+  <si>
     <t>CORRECTIONAL ITEMS</t>
   </si>
   <si>
+    <t>New frosted panel has a crack. Needs to be replaced.</t>
+  </si>
+  <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>All punchwork need to be performed during off-hours.</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1116,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>999999</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1104,62 +1140,86 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="25"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="29"/>
+      <c r="A8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="30">
+        <v>2</v>
+      </c>
+      <c r="D8" s="31">
+        <v>4</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="34"/>
+      <c r="A9" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="35">
+        <v>2</v>
+      </c>
+      <c r="D9" s="36">
+        <v>4</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="L9" s="38"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1272,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="41">
@@ -1228,7 +1288,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -1239,7 +1299,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
@@ -1275,7 +1335,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -1286,7 +1346,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
@@ -1321,7 +1381,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>
@@ -1332,7 +1392,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>

</xml_diff>

<commit_message>
summary task view on click
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>MacArthur Park New Restroom</t>
+    <t>Sneeze Partition Installation</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>06/07/2021</t>
+    <t>05/03/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>30J0049.00</t>
+    <t>9055-017.00.01</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,13 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t/>
+    <t>07:00</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
+    <t>Sunny</t>
+  </si>
+  <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>16:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -83,19 +89,49 @@
 /Day</t>
   </si>
   <si>
+    <t>Exbon Development Inc.</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Forklift</t>
+  </si>
+  <si>
+    <t>JPUS</t>
+  </si>
+  <si>
+    <t>Laborer</t>
+  </si>
+  <si>
+    <t>Dump Truck</t>
+  </si>
+  <si>
+    <t>Existing Partition Removal</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>0</t>
+    <t>4</t>
   </si>
   <si>
     <t>TESTS &amp; INSPECTIONS</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspection is scheduled on May 4, 2021 at 3PM. </t>
+  </si>
+  <si>
     <t>CORRECTIONAL ITEMS</t>
   </si>
   <si>
+    <t>New frosted panel has a crack. Needs to be replaced.</t>
+  </si>
+  <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>All punchwork need to be performed during off-hours.</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>6249</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1101,62 +1137,86 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="36.75" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="24"/>
     </row>
     <row r="8" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="28"/>
+      <c r="A8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30">
+        <v>4</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" ht="21" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="33"/>
+      <c r="A9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="34">
+        <v>2</v>
+      </c>
+      <c r="D9" s="35">
+        <v>4</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="L9" s="37"/>
     </row>
     <row r="10" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1209,11 +1269,11 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B16" s="39"/>
       <c r="C16" s="40" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="21"/>
@@ -1224,7 +1284,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -1235,7 +1295,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -1271,7 +1331,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -1282,7 +1342,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -1317,7 +1377,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -1328,7 +1388,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>